<commit_message>
restitution jour, semaine, mois N°1
</commit_message>
<xml_diff>
--- a/data/pointage.xlsx
+++ b/data/pointage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJETS\POINTAGE\POINTAGE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFB6395-8E34-4061-9F5B-6852A4D0D8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1510CAE2-119D-478D-8F01-C9E4EF2486CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,7 +112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -123,7 +123,6 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,7 +341,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -396,7 +395,7 @@
       <c r="E2" s="5">
         <v>1</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="5">

</xml_diff>